<commit_message>
biso new unit tests with full heterogeneous hcpb
</commit_message>
<xml_diff>
--- a/Jupyter/data_combined.xlsx
+++ b/Jupyter/data_combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCNP\emma-openmc\Jupyter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500CD8E6-2BEC-4EF0-BC21-0E33E512F863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B288F2B9-F472-443E-84BD-6D56C5E73574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1992" yWindow="1224" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
   <si>
     <t>Breeder</t>
   </si>
@@ -95,7 +95,10 @@
     <t>Pb-17Li</t>
   </si>
   <si>
-    <t>Li4SiO4-Be pebble bed</t>
+    <t>Li4SiO4-Be-He</t>
+  </si>
+  <si>
+    <t>Li4SiO4-Be</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,7 +941,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -978,7 +981,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1006,7 +1009,7 @@
     </row>
     <row r="17" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="5">
         <v>50</v>
@@ -1046,7 +1049,7 @@
     </row>
     <row r="18" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" s="5">
         <v>50</v>
@@ -1094,14 +1097,14 @@
         <v>6.2325669999999991E-6</v>
       </c>
       <c r="G19" s="11">
-        <v>2724.22</v>
+        <v>2743.65</v>
       </c>
       <c r="H19" s="11">
         <v>3834.44</v>
       </c>
       <c r="I19" s="12">
         <f>E19*G19</f>
-        <v>1.6978883672739996E-2</v>
+        <v>1.7099982449549998E-2</v>
       </c>
       <c r="J19" s="12">
         <f>F19*H19</f>
@@ -1109,7 +1112,7 @@
       </c>
       <c r="K19" s="13">
         <f t="shared" ref="K19:K22" si="1">(J19-I19)/(I19)*100</f>
-        <v>40.753683623202249</v>
+        <v>39.756893189729006</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1132,10 +1135,7 @@
       <c r="J20" s="10">
         <v>2.3854150630574E-2</v>
       </c>
-      <c r="K20" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K20" s="13"/>
     </row>
     <row r="21" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
@@ -1159,22 +1159,22 @@
         <v>6.2325669999999991E-6</v>
       </c>
       <c r="G21" s="15">
-        <v>84061.5</v>
+        <v>93396</v>
       </c>
       <c r="H21" s="15">
-        <v>101466</v>
+        <v>101228</v>
       </c>
       <c r="I21" s="16">
         <f>E21*G21</f>
-        <v>0.5239189308704999</v>
+        <v>0.58209682753199987</v>
       </c>
       <c r="J21" s="16">
         <f>F21*H21</f>
-        <v>0.63239364322199987</v>
+        <v>0.63091029227599993</v>
       </c>
       <c r="K21" s="17">
         <f t="shared" si="1"/>
-        <v>20.704484216912615</v>
+        <v>8.3857981069853214</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1197,10 +1197,7 @@
       <c r="J22" s="14">
         <v>0.63221071094595604</v>
       </c>
-      <c r="K22" s="17" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="K22" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>